<commit_message>
Company changes - 28 Mar 2023
</commit_message>
<xml_diff>
--- a/TestData/T1144_T1146_Companies_AddNewCompanyWithRecordTypeForCapitalProviderAndOperatingCompany.xlsx
+++ b/TestData/T1144_T1146_Companies_AddNewCompanyWithRecordTypeForCapitalProviderAndOperatingCompany.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20387"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26130"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SMittal0207\source\repos\SalesForce_Project\TestData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SMittal0207\source\repos\SF_Automation\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E2E8452-7BB7-4255-9987-5C93A4BA8E2E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93DAEB65-18A1-4A31-9C11-069887FD001E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="7536" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Company" sheetId="1" r:id="rId1"/>
@@ -110,9 +110,6 @@
     <t>Capital Provider</t>
   </si>
   <si>
-    <t>TestCapitalProvider</t>
-  </si>
-  <si>
     <t>Asset Manager</t>
   </si>
   <si>
@@ -156,6 +153,9 @@
   </si>
   <si>
     <t>Archived Accounts</t>
+  </si>
+  <si>
+    <t>TestNewCapitalProvider</t>
   </si>
 </sst>
 </file>
@@ -199,17 +199,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -492,8 +490,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -550,8 +548,8 @@
       <c r="M1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="N1" s="2" t="s">
-        <v>30</v>
+      <c r="N1" s="1" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.3">
@@ -559,7 +557,7 @@
         <v>26</v>
       </c>
       <c r="B2" t="s">
-        <v>27</v>
+        <v>42</v>
       </c>
       <c r="C2" t="s">
         <v>12</v>
@@ -580,7 +578,7 @@
         <v>17</v>
       </c>
       <c r="I2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="J2" t="s">
         <v>19</v>
@@ -594,8 +592,8 @@
       <c r="M2" t="s">
         <v>25</v>
       </c>
-      <c r="N2" s="3" t="s">
-        <v>31</v>
+      <c r="N2" s="2" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.3">
@@ -615,7 +613,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
@@ -628,32 +626,32 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>36</v>
-      </c>
       <c r="C1" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" s="5" t="s">
+      <c r="A2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B2" t="s">
         <v>41</v>
       </c>
-      <c r="B2" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>41</v>
+      <c r="C2" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>26</v>
       </c>
-      <c r="B3" s="4" t="s">
-        <v>37</v>
+      <c r="B3" s="3" t="s">
+        <v>36</v>
       </c>
       <c r="C3" t="s">
         <v>2</v>
@@ -661,10 +659,10 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C4" t="s">
         <v>26</v>
@@ -672,35 +670,35 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>2</v>
       </c>
-      <c r="B7" s="4" t="s">
-        <v>40</v>
+      <c r="B7" s="3" t="s">
+        <v>39</v>
       </c>
       <c r="C7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
   </sheetData>
@@ -729,7 +727,7 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Revert "Company changes - 28 Mar 2023"
This reverts commit 9c386bba6aa2ca7d61f78ff06ebbc178869eba92.
</commit_message>
<xml_diff>
--- a/TestData/T1144_T1146_Companies_AddNewCompanyWithRecordTypeForCapitalProviderAndOperatingCompany.xlsx
+++ b/TestData/T1144_T1146_Companies_AddNewCompanyWithRecordTypeForCapitalProviderAndOperatingCompany.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20387"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SMittal0207\source\repos\SF_Automation\TestData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SMittal0207\source\repos\SalesForce_Project\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93DAEB65-18A1-4A31-9C11-069887FD001E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E2E8452-7BB7-4255-9987-5C93A4BA8E2E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="7536" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Company" sheetId="1" r:id="rId1"/>
@@ -110,6 +110,9 @@
     <t>Capital Provider</t>
   </si>
   <si>
+    <t>TestCapitalProvider</t>
+  </si>
+  <si>
     <t>Asset Manager</t>
   </si>
   <si>
@@ -153,9 +156,6 @@
   </si>
   <si>
     <t>Archived Accounts</t>
-  </si>
-  <si>
-    <t>TestNewCapitalProvider</t>
   </si>
 </sst>
 </file>
@@ -199,15 +199,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -490,8 +492,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -548,8 +550,8 @@
       <c r="M1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="N1" s="1" t="s">
-        <v>29</v>
+      <c r="N1" s="2" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.3">
@@ -557,7 +559,7 @@
         <v>26</v>
       </c>
       <c r="B2" t="s">
-        <v>42</v>
+        <v>27</v>
       </c>
       <c r="C2" t="s">
         <v>12</v>
@@ -578,7 +580,7 @@
         <v>17</v>
       </c>
       <c r="I2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="J2" t="s">
         <v>19</v>
@@ -592,8 +594,8 @@
       <c r="M2" t="s">
         <v>25</v>
       </c>
-      <c r="N2" s="2" t="s">
-        <v>30</v>
+      <c r="N2" s="3" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.3">
@@ -613,7 +615,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
@@ -626,32 +628,32 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>34</v>
-      </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>40</v>
-      </c>
-      <c r="B2" t="s">
+      <c r="A2" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="C2" t="s">
-        <v>40</v>
+      <c r="B2" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>26</v>
       </c>
-      <c r="B3" s="3" t="s">
-        <v>36</v>
+      <c r="B3" s="4" t="s">
+        <v>37</v>
       </c>
       <c r="C3" t="s">
         <v>2</v>
@@ -659,10 +661,10 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B4" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C4" t="s">
         <v>26</v>
@@ -670,35 +672,35 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
+        <v>33</v>
+      </c>
+      <c r="B5" t="s">
+        <v>38</v>
+      </c>
+      <c r="C5" t="s">
         <v>32</v>
-      </c>
-      <c r="B5" t="s">
-        <v>37</v>
-      </c>
-      <c r="C5" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
+        <v>34</v>
+      </c>
+      <c r="B6" t="s">
+        <v>39</v>
+      </c>
+      <c r="C6" t="s">
         <v>33</v>
-      </c>
-      <c r="B6" t="s">
-        <v>38</v>
-      </c>
-      <c r="C6" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>2</v>
       </c>
-      <c r="B7" s="3" t="s">
-        <v>39</v>
+      <c r="B7" s="4" t="s">
+        <v>40</v>
       </c>
       <c r="C7" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>
@@ -727,7 +729,7 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Contacts & Companies - 29th Mar 2023
</commit_message>
<xml_diff>
--- a/TestData/T1144_T1146_Companies_AddNewCompanyWithRecordTypeForCapitalProviderAndOperatingCompany.xlsx
+++ b/TestData/T1144_T1146_Companies_AddNewCompanyWithRecordTypeForCapitalProviderAndOperatingCompany.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20387"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26130"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SMittal0207\source\repos\SalesForce_Project\TestData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SMittal0207\source\repos\SF_Automation\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E2E8452-7BB7-4255-9987-5C93A4BA8E2E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0B3437D-3CEB-4F51-9F24-C02241D08BC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="7536" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Company" sheetId="1" r:id="rId1"/>
@@ -110,9 +110,6 @@
     <t>Capital Provider</t>
   </si>
   <si>
-    <t>TestCapitalProvider</t>
-  </si>
-  <si>
     <t>Asset Manager</t>
   </si>
   <si>
@@ -156,6 +153,9 @@
   </si>
   <si>
     <t>Archived Accounts</t>
+  </si>
+  <si>
+    <t>TestNewCapitalProvider</t>
   </si>
 </sst>
 </file>
@@ -199,17 +199,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -492,8 +490,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -550,8 +548,8 @@
       <c r="M1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="N1" s="2" t="s">
-        <v>30</v>
+      <c r="N1" s="1" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.3">
@@ -559,7 +557,7 @@
         <v>26</v>
       </c>
       <c r="B2" t="s">
-        <v>27</v>
+        <v>42</v>
       </c>
       <c r="C2" t="s">
         <v>12</v>
@@ -580,7 +578,7 @@
         <v>17</v>
       </c>
       <c r="I2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="J2" t="s">
         <v>19</v>
@@ -594,8 +592,8 @@
       <c r="M2" t="s">
         <v>25</v>
       </c>
-      <c r="N2" s="3" t="s">
-        <v>31</v>
+      <c r="N2" s="2" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.3">
@@ -615,7 +613,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
@@ -628,32 +626,32 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>36</v>
-      </c>
       <c r="C1" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" s="5" t="s">
+      <c r="A2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B2" t="s">
         <v>41</v>
       </c>
-      <c r="B2" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>41</v>
+      <c r="C2" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>26</v>
       </c>
-      <c r="B3" s="4" t="s">
-        <v>37</v>
+      <c r="B3" s="3" t="s">
+        <v>36</v>
       </c>
       <c r="C3" t="s">
         <v>2</v>
@@ -661,10 +659,10 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C4" t="s">
         <v>26</v>
@@ -672,35 +670,35 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>2</v>
       </c>
-      <c r="B7" s="4" t="s">
-        <v>40</v>
+      <c r="B7" s="3" t="s">
+        <v>39</v>
       </c>
       <c r="C7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
   </sheetData>
@@ -729,7 +727,7 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Companies Changes 1 - 29th June 2023
</commit_message>
<xml_diff>
--- a/TestData/T1144_T1146_Companies_AddNewCompanyWithRecordTypeForCapitalProviderAndOperatingCompany.xlsx
+++ b/TestData/T1144_T1146_Companies_AddNewCompanyWithRecordTypeForCapitalProviderAndOperatingCompany.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26501"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SMittal0207\source\repos\SF_Automation\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0B3437D-3CEB-4F51-9F24-C02241D08BC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{043EFF70-5C15-41F1-9DEF-562D6C51FB95}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Company" sheetId="1" r:id="rId1"/>
@@ -113,9 +113,6 @@
     <t>Asset Manager</t>
   </si>
   <si>
-    <t>Nicole Bicho</t>
-  </si>
-  <si>
     <t>Postal Code</t>
   </si>
   <si>
@@ -156,6 +153,9 @@
   </si>
   <si>
     <t>TestNewCapitalProvider</t>
+  </si>
+  <si>
+    <t>Drew Koecher</t>
   </si>
 </sst>
 </file>
@@ -490,7 +490,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -549,7 +549,7 @@
         <v>24</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.3">
@@ -557,7 +557,7 @@
         <v>26</v>
       </c>
       <c r="B2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C2" t="s">
         <v>12</v>
@@ -593,7 +593,7 @@
         <v>25</v>
       </c>
       <c r="N2" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.3">
@@ -626,24 +626,24 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>35</v>
-      </c>
       <c r="C1" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B2" t="s">
         <v>40</v>
       </c>
-      <c r="B2" t="s">
-        <v>41</v>
-      </c>
       <c r="C2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
@@ -651,7 +651,7 @@
         <v>26</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C3" t="s">
         <v>2</v>
@@ -659,10 +659,10 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C4" t="s">
         <v>26</v>
@@ -670,24 +670,24 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="100.8" x14ac:dyDescent="0.3">
@@ -695,10 +695,10 @@
         <v>2</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -711,8 +711,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N18" sqref="N18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -727,7 +727,7 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>28</v>
+        <v>42</v>
       </c>
     </row>
   </sheetData>

</xml_diff>